<commit_message>
Closed #79. TOTAL  571,469
</commit_message>
<xml_diff>
--- a/Zara.Reto0/ZaraCalculos.xlsx
+++ b/Zara.Reto0/ZaraCalculos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\source\repos\Zara.Reto0\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -151,7 +151,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -375,7 +375,7 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2"/>
@@ -386,14 +386,16 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="5" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="9" borderId="4" xfId="7" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="9" borderId="4" xfId="7" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="6" borderId="1" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="5" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="8" fillId="8" borderId="3" xfId="6" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="1" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="8" borderId="3" xfId="6" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="7" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Bad" xfId="4" builtinId="27"/>
@@ -683,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -829,18 +831,24 @@
       <c r="L3" s="1">
         <v>64.349000000000004</v>
       </c>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
+      <c r="M3" s="18">
+        <v>30</v>
+      </c>
+      <c r="N3" s="11">
+        <v>1.8580000000000001</v>
+      </c>
+      <c r="O3" s="19">
+        <v>26.375</v>
+      </c>
       <c r="P3" s="11">
-        <f>N3*29.17</f>
-        <v>0</v>
+        <f t="shared" ref="P3:P14" si="0">N3*29.17</f>
+        <v>54.197860000000006</v>
       </c>
       <c r="Q3" s="10"/>
       <c r="R3" s="10"/>
       <c r="S3" s="10"/>
       <c r="T3" s="10">
-        <f>R3*29.17</f>
+        <f t="shared" ref="T3:T14" si="1">R3*29.17</f>
         <v>0</v>
       </c>
     </row>
@@ -878,18 +886,24 @@
       <c r="L4" s="1">
         <v>68.783000000000001</v>
       </c>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
+      <c r="M4" s="18">
+        <v>27</v>
+      </c>
+      <c r="N4" s="11">
+        <v>1.7569999999999999</v>
+      </c>
+      <c r="O4" s="19">
+        <v>27.885000000000002</v>
+      </c>
       <c r="P4" s="11">
-        <f>N4*29.17</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>51.251689999999996</v>
       </c>
       <c r="Q4" s="10"/>
       <c r="R4" s="10"/>
       <c r="S4" s="10"/>
       <c r="T4" s="10">
-        <f>R4*29.17</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -927,18 +941,24 @@
       <c r="L5" s="1">
         <v>64.290999999999997</v>
       </c>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
+      <c r="M5" s="18">
+        <v>27</v>
+      </c>
+      <c r="N5" s="11">
+        <v>1.65</v>
+      </c>
+      <c r="O5" s="19">
+        <v>29.7</v>
+      </c>
       <c r="P5" s="11">
-        <f>N5*29.17</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>48.130499999999998</v>
       </c>
       <c r="Q5" s="10"/>
       <c r="R5" s="10"/>
       <c r="S5" s="10"/>
       <c r="T5" s="10">
-        <f>R5*29.17</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -972,18 +992,24 @@
       <c r="L6" s="1">
         <v>66.741</v>
       </c>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
+      <c r="M6" s="18">
+        <v>4</v>
+      </c>
+      <c r="N6" s="11">
+        <v>1.7090000000000001</v>
+      </c>
+      <c r="O6" s="19">
+        <v>28.664999999999999</v>
+      </c>
       <c r="P6" s="11">
-        <f>N6*29.17</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>49.851530000000004</v>
       </c>
       <c r="Q6" s="10"/>
       <c r="R6" s="10"/>
       <c r="S6" s="10"/>
       <c r="T6" s="10">
-        <f>R6*29.17</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1015,21 +1041,27 @@
         <v>21.2</v>
       </c>
       <c r="L7" s="10">
-        <f>J7*29.17</f>
+        <f t="shared" ref="L7:L14" si="2">J7*29.17</f>
         <v>67.411870000000008</v>
       </c>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11"/>
+      <c r="M7" s="18">
+        <v>29</v>
+      </c>
+      <c r="N7" s="11">
+        <v>1.5980000000000001</v>
+      </c>
+      <c r="O7" s="19">
+        <v>30.655000000000001</v>
+      </c>
       <c r="P7" s="11">
-        <f>N7*29.17</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>46.613660000000003</v>
       </c>
       <c r="Q7" s="10"/>
       <c r="R7" s="10"/>
       <c r="S7" s="10"/>
       <c r="T7" s="10">
-        <f>R7*29.17</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1061,21 +1093,27 @@
         <v>22.59</v>
       </c>
       <c r="L8" s="10">
-        <f>J8*29.17</f>
+        <f t="shared" si="2"/>
         <v>63.269730000000003</v>
       </c>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
+      <c r="M8" s="18">
+        <v>26</v>
+      </c>
+      <c r="N8" s="11">
+        <v>1.6240000000000001</v>
+      </c>
+      <c r="O8" s="19">
+        <v>30.164999999999999</v>
+      </c>
       <c r="P8" s="11">
-        <f>N8*29.17</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>47.372080000000004</v>
       </c>
       <c r="Q8" s="10"/>
       <c r="R8" s="10"/>
       <c r="S8" s="10"/>
       <c r="T8" s="10">
-        <f>R8*29.17</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1105,21 +1143,27 @@
         <v>21.914999999999999</v>
       </c>
       <c r="L9" s="10">
-        <f>J9*29.17</f>
+        <f t="shared" si="2"/>
         <v>65.224120000000013</v>
       </c>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
+      <c r="M9" s="18">
+        <v>31</v>
+      </c>
+      <c r="N9" s="11">
+        <v>1.5920000000000001</v>
+      </c>
+      <c r="O9" s="19">
+        <v>30.785</v>
+      </c>
       <c r="P9" s="11">
-        <f>N9*29.17</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>46.438640000000007</v>
       </c>
       <c r="Q9" s="10"/>
       <c r="R9" s="10"/>
       <c r="S9" s="10"/>
       <c r="T9" s="10">
-        <f>R9*29.17</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1149,21 +1193,27 @@
         <v>22.18</v>
       </c>
       <c r="L10" s="10">
-        <f>J10*29.17</f>
+        <f t="shared" si="2"/>
         <v>64.436530000000005</v>
       </c>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="11"/>
+      <c r="M10" s="18">
+        <v>28</v>
+      </c>
+      <c r="N10" s="11">
+        <v>1.6419999999999999</v>
+      </c>
+      <c r="O10" s="19">
+        <v>29.85</v>
+      </c>
       <c r="P10" s="11">
-        <f>N10*29.17</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>47.89714</v>
       </c>
       <c r="Q10" s="10"/>
       <c r="R10" s="10"/>
       <c r="S10" s="10"/>
       <c r="T10" s="10">
-        <f>R10*29.17</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1193,21 +1243,27 @@
         <v>21.88</v>
       </c>
       <c r="L11" s="10">
-        <f>J11*29.17</f>
+        <f t="shared" si="2"/>
         <v>65.311629999999994</v>
       </c>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="11"/>
+      <c r="M11" s="18">
+        <v>25</v>
+      </c>
+      <c r="N11" s="11">
+        <v>1.6990000000000001</v>
+      </c>
+      <c r="O11" s="19">
+        <v>28.84</v>
+      </c>
       <c r="P11" s="11">
-        <f>N11*29.17</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>49.559830000000005</v>
       </c>
       <c r="Q11" s="10"/>
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
       <c r="T11" s="10">
-        <f>R11*29.17</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1237,21 +1293,27 @@
         <v>22.15</v>
       </c>
       <c r="L12" s="10">
-        <f>J12*29.17</f>
+        <f t="shared" si="2"/>
         <v>64.524040000000014</v>
       </c>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="11"/>
+      <c r="M12" s="18">
+        <v>30</v>
+      </c>
+      <c r="N12" s="11">
+        <v>1.42</v>
+      </c>
+      <c r="O12" s="19">
+        <v>34.5</v>
+      </c>
       <c r="P12" s="11">
-        <f>N12*29.17</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>41.421399999999998</v>
       </c>
       <c r="Q12" s="10"/>
       <c r="R12" s="10"/>
       <c r="S12" s="10"/>
       <c r="T12" s="10">
-        <f>R12*29.17</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1281,21 +1343,27 @@
         <v>23.225000000000001</v>
       </c>
       <c r="L13" s="10">
-        <f>J13*29.17</f>
+        <f t="shared" si="2"/>
         <v>61.548699999999997</v>
       </c>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="11"/>
+      <c r="M13" s="18">
+        <v>27</v>
+      </c>
+      <c r="N13" s="11">
+        <v>1.48</v>
+      </c>
+      <c r="O13" s="19">
+        <v>33.115000000000002</v>
+      </c>
       <c r="P13" s="11">
-        <f>N13*29.17</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>43.171600000000005</v>
       </c>
       <c r="Q13" s="10"/>
       <c r="R13" s="10"/>
       <c r="S13" s="10"/>
       <c r="T13" s="10">
-        <f>R13*29.17</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1325,21 +1393,27 @@
         <v>23.82</v>
       </c>
       <c r="L14" s="10">
-        <f>J14*29.17</f>
+        <f t="shared" si="2"/>
         <v>60.002690000000001</v>
       </c>
-      <c r="M14" s="11"/>
-      <c r="N14" s="11"/>
-      <c r="O14" s="11"/>
+      <c r="M14" s="18">
+        <v>4</v>
+      </c>
+      <c r="N14" s="11">
+        <v>1.5620000000000001</v>
+      </c>
+      <c r="O14" s="19">
+        <v>31.364999999999998</v>
+      </c>
       <c r="P14" s="11">
-        <f>N14*29.17</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>45.563540000000003</v>
       </c>
       <c r="Q14" s="10"/>
       <c r="R14" s="10"/>
       <c r="S14" s="10"/>
       <c r="T14" s="10">
-        <f>R14*29.17</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1374,12 +1448,12 @@
       <c r="M15" s="11"/>
       <c r="N15" s="11">
         <f>SUM(N3:N14)</f>
-        <v>0</v>
+        <v>19.591000000000001</v>
       </c>
       <c r="O15" s="11"/>
       <c r="P15" s="11">
         <f>SUM(P3:P14)</f>
-        <v>0</v>
+        <v>571.46947</v>
       </c>
       <c r="Q15" s="10"/>
       <c r="R15" s="10">
@@ -1402,10 +1476,12 @@
       <c r="C16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="10"/>
+      <c r="D16" s="14">
+        <v>571.46900000000005</v>
+      </c>
       <c r="E16" s="10"/>
       <c r="F16" s="5">
-        <v>571.471</v>
+        <v>571.46900000000005</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1450,7 +1526,7 @@
       <c r="C19" s="5"/>
       <c r="D19" s="15">
         <f>SUM(D2:D18)</f>
-        <v>16504.73335459701</v>
+        <v>17076.202354597011</v>
       </c>
       <c r="E19" s="15">
         <f>SUM(E2:E18)</f>

</xml_diff>

<commit_message>
Añadidos valores de Genis. Correctos!
</commit_message>
<xml_diff>
--- a/Zara.Reto0/ZaraCalculos.xlsx
+++ b/Zara.Reto0/ZaraCalculos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="41">
   <si>
     <t>Nombre</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>SI</t>
+  </si>
+  <si>
+    <t>Si</t>
   </si>
 </sst>
 </file>
@@ -686,7 +689,7 @@
   <dimension ref="A1:T34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -759,7 +762,9 @@
         <v>14</v>
       </c>
       <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="E2" s="14">
+        <v>2992.6669999999999</v>
+      </c>
       <c r="F2" s="5"/>
       <c r="H2" s="2" t="s">
         <v>21</v>
@@ -1127,7 +1132,9 @@
       <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="10"/>
+      <c r="D9" s="14">
+        <v>2764.7620000000002</v>
+      </c>
       <c r="E9" s="10"/>
       <c r="F9" s="5"/>
       <c r="H9" s="7" t="s">
@@ -1178,7 +1185,9 @@
         <v>14</v>
       </c>
       <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
+      <c r="E10" s="14">
+        <v>2473.3829999999998</v>
+      </c>
       <c r="F10" s="5"/>
       <c r="H10" s="7" t="s">
         <v>31</v>
@@ -1526,11 +1535,11 @@
       <c r="C19" s="5"/>
       <c r="D19" s="15">
         <f>SUM(D2:D18)</f>
-        <v>17076.202354597011</v>
+        <v>19840.96435459701</v>
       </c>
       <c r="E19" s="15">
         <f>SUM(E2:E18)</f>
-        <v>14935.080923935813</v>
+        <v>20401.130923935816</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
@@ -1590,7 +1599,9 @@
       <c r="A29" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B29" s="17"/>
+      <c r="B29" s="16" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">

</xml_diff>

<commit_message>
Closed #61, closed #62, closed #65, closed #66, closed #75
</commit_message>
<xml_diff>
--- a/Zara.Reto0/ZaraCalculos.xlsx
+++ b/Zara.Reto0/ZaraCalculos.xlsx
@@ -156,7 +156,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,6 +238,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -288,7 +296,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -367,8 +375,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
@@ -377,8 +394,9 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2"/>
@@ -399,11 +417,13 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="7" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="8"/>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
     <cellStyle name="Bad" xfId="4" builtinId="27"/>
     <cellStyle name="Check Cell" xfId="6" builtinId="23"/>
     <cellStyle name="Good" xfId="3" builtinId="26"/>
+    <cellStyle name="Heading 1" xfId="8" builtinId="16"/>
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Neutral" xfId="5" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -688,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -761,11 +781,15 @@
       <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="10"/>
+      <c r="D2" s="14">
+        <v>2992.6669999999999</v>
+      </c>
       <c r="E2" s="14">
         <v>2992.6669999999999</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="5">
+        <v>2992.6669999999999</v>
+      </c>
       <c r="H2" s="2" t="s">
         <v>21</v>
       </c>
@@ -816,11 +840,15 @@
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="13">
         <v>3987.567</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="5"/>
+      <c r="E3" s="14">
+        <v>3987.1309999999999</v>
+      </c>
+      <c r="F3" s="5">
+        <v>3987.1309999999999</v>
+      </c>
       <c r="H3" s="7" t="s">
         <v>24</v>
       </c>
@@ -867,8 +895,8 @@
       <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="13">
-        <v>4376.3109999999997</v>
+      <c r="D4" s="14">
+        <v>4352.4849999999997</v>
       </c>
       <c r="E4" s="13">
         <v>4341.1379999999999</v>
@@ -922,11 +950,11 @@
       <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="13">
         <v>4500.7887341804799</v>
       </c>
-      <c r="E5" s="13">
-        <v>4538.5240000000003</v>
+      <c r="E5" s="14">
+        <v>4500.8140000000003</v>
       </c>
       <c r="F5" s="5">
         <v>4500.8140000000003</v>
@@ -977,11 +1005,15 @@
       <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10">
-        <v>3667.4789239358129</v>
-      </c>
-      <c r="F6" s="5"/>
+      <c r="D6" s="14">
+        <v>3667.5149999999999</v>
+      </c>
+      <c r="E6" s="13">
+        <v>3667.4789239358101</v>
+      </c>
+      <c r="F6" s="5">
+        <v>3667.5149999999999</v>
+      </c>
       <c r="H6" s="7" t="s">
         <v>27</v>
       </c>
@@ -1028,11 +1060,15 @@
       <c r="C7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="13">
         <v>2375.08</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="5"/>
+      <c r="E7" s="14">
+        <v>2558.9969999999998</v>
+      </c>
+      <c r="F7" s="5">
+        <v>2558.9969999999998</v>
+      </c>
       <c r="H7" s="7" t="s">
         <v>28</v>
       </c>
@@ -1081,10 +1117,12 @@
         <v>12</v>
       </c>
       <c r="D8" s="10"/>
-      <c r="E8" s="10">
+      <c r="E8" s="13">
         <v>1902.347</v>
       </c>
-      <c r="F8" s="5"/>
+      <c r="F8" s="5">
+        <v>1902.38</v>
+      </c>
       <c r="H8" s="7" t="s">
         <v>29</v>
       </c>
@@ -1136,7 +1174,9 @@
         <v>2764.7620000000002</v>
       </c>
       <c r="E9" s="10"/>
-      <c r="F9" s="5"/>
+      <c r="F9" s="5">
+        <v>2764.7620000000002</v>
+      </c>
       <c r="H9" s="7" t="s">
         <v>30</v>
       </c>
@@ -1188,7 +1228,9 @@
       <c r="E10" s="14">
         <v>2473.3829999999998</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="5">
+        <v>2473.3829999999998</v>
+      </c>
       <c r="H10" s="7" t="s">
         <v>31</v>
       </c>
@@ -1238,7 +1280,9 @@
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
-      <c r="F11" s="5"/>
+      <c r="F11" s="5">
+        <v>1697.8689999999999</v>
+      </c>
       <c r="H11" s="7" t="s">
         <v>32</v>
       </c>
@@ -1287,8 +1331,12 @@
         <v>9</v>
       </c>
       <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="5"/>
+      <c r="E12" s="14">
+        <v>1420.316</v>
+      </c>
+      <c r="F12" s="5">
+        <v>1420.316</v>
+      </c>
       <c r="H12" s="7" t="s">
         <v>33</v>
       </c>
@@ -1338,7 +1386,9 @@
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
-      <c r="F13" s="5"/>
+      <c r="F13" s="5">
+        <v>1060.825</v>
+      </c>
       <c r="H13" s="7" t="s">
         <v>34</v>
       </c>
@@ -1388,7 +1438,9 @@
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
-      <c r="F14" s="5"/>
+      <c r="F14" s="5">
+        <v>812.09299999999996</v>
+      </c>
       <c r="H14" s="7" t="s">
         <v>35</v>
       </c>
@@ -1440,7 +1492,9 @@
         <v>775.89331000000016</v>
       </c>
       <c r="E15" s="10"/>
-      <c r="F15" s="5"/>
+      <c r="F15" s="5">
+        <v>775.89300000000003</v>
+      </c>
       <c r="H15" s="2" t="s">
         <v>20</v>
       </c>
@@ -1488,7 +1542,9 @@
       <c r="D16" s="14">
         <v>571.46900000000005</v>
       </c>
-      <c r="E16" s="10"/>
+      <c r="E16" s="14">
+        <v>571.46900000000005</v>
+      </c>
       <c r="F16" s="5">
         <v>571.46900000000005</v>
       </c>
@@ -1505,7 +1561,9 @@
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
-      <c r="F17" s="5"/>
+      <c r="F17" s="5">
+        <v>561.37699999999995</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
@@ -1527,7 +1585,7 @@
         <v>485.59300000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="5" t="s">
         <v>20</v>
       </c>
@@ -1535,11 +1593,14 @@
       <c r="C19" s="5"/>
       <c r="D19" s="15">
         <f>SUM(D2:D18)</f>
-        <v>19840.96435459701</v>
+        <v>26477.32035459701</v>
       </c>
       <c r="E19" s="15">
         <f>SUM(E2:E18)</f>
-        <v>20401.130923935816</v>
+        <v>28901.333923935814</v>
+      </c>
+      <c r="F19" s="20">
+        <v>36585.567999999999</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Closed #67, Closed #69, Closed #68, Closed #71, Closed #73, Closed #74, Closed #76. Años 2010 y 2012, ISSUES #70 y #72 no completados por Josep pasado el tiempo límite
</commit_message>
<xml_diff>
--- a/Zara.Reto0/ZaraCalculos.xlsx
+++ b/Zara.Reto0/ZaraCalculos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="45">
   <si>
     <t>Nombre</t>
   </si>
@@ -149,10 +149,16 @@
     <t>Si</t>
   </si>
   <si>
+    <t>NO</t>
+  </si>
+  <si>
     <t>Correcto</t>
   </si>
   <si>
     <t>Incorrecto</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -402,7 +408,7 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2"/>
@@ -412,7 +418,6 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="5" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="5" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="16" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="9" borderId="4" xfId="7" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="1" applyFill="1" applyBorder="1"/>
@@ -426,6 +431,8 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="8"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="4" xfId="3" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Bad" xfId="4" builtinId="27"/>
@@ -716,8 +723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -756,7 +763,7 @@
       <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>38</v>
       </c>
       <c r="H1" s="8"/>
@@ -783,10 +790,10 @@
       <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="13">
         <v>2992.6669999999999</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="13">
         <v>2992.6669999999999</v>
       </c>
       <c r="F2" s="5">
@@ -830,10 +837,10 @@
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="12">
         <v>3987.567</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="13">
         <v>3987.1309999999999</v>
       </c>
       <c r="F3" s="5">
@@ -854,16 +861,16 @@
       <c r="L3" s="1">
         <v>64.349000000000004</v>
       </c>
-      <c r="M3" s="18">
+      <c r="M3" s="17">
         <v>30</v>
       </c>
-      <c r="N3" s="11">
+      <c r="N3" s="10">
         <v>1.8580000000000001</v>
       </c>
-      <c r="O3" s="19">
+      <c r="O3" s="18">
         <v>26.375</v>
       </c>
-      <c r="P3" s="11">
+      <c r="P3" s="10">
         <f t="shared" ref="P3:P14" si="0">N3*29.17</f>
         <v>54.197860000000006</v>
       </c>
@@ -878,10 +885,10 @@
       <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="13">
         <v>4352.4849999999997</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="12">
         <v>4341.1379999999999</v>
       </c>
       <c r="F4" s="5">
@@ -902,16 +909,16 @@
       <c r="L4" s="1">
         <v>68.783000000000001</v>
       </c>
-      <c r="M4" s="18">
+      <c r="M4" s="17">
         <v>27</v>
       </c>
-      <c r="N4" s="11">
+      <c r="N4" s="10">
         <v>1.7569999999999999</v>
       </c>
-      <c r="O4" s="19">
+      <c r="O4" s="18">
         <v>27.885000000000002</v>
       </c>
-      <c r="P4" s="11">
+      <c r="P4" s="10">
         <f t="shared" si="0"/>
         <v>51.251689999999996</v>
       </c>
@@ -927,9 +934,9 @@
         <v>9</v>
       </c>
       <c r="D5" s="13">
-        <v>4500.7887341804799</v>
-      </c>
-      <c r="E5" s="14">
+        <v>4500.8140000000003</v>
+      </c>
+      <c r="E5" s="13">
         <v>4500.8140000000003</v>
       </c>
       <c r="F5" s="5">
@@ -950,16 +957,16 @@
       <c r="L5" s="1">
         <v>64.290999999999997</v>
       </c>
-      <c r="M5" s="18">
+      <c r="M5" s="17">
         <v>27</v>
       </c>
-      <c r="N5" s="11">
+      <c r="N5" s="10">
         <v>1.65</v>
       </c>
-      <c r="O5" s="19">
+      <c r="O5" s="18">
         <v>29.7</v>
       </c>
-      <c r="P5" s="11">
+      <c r="P5" s="10">
         <f t="shared" si="0"/>
         <v>48.130499999999998</v>
       </c>
@@ -974,11 +981,11 @@
       <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="13">
         <v>3667.5149999999999</v>
       </c>
       <c r="E6" s="13">
-        <v>3667.4789239358101</v>
+        <v>3667.5149999999999</v>
       </c>
       <c r="F6" s="5">
         <v>3667.5149999999999</v>
@@ -998,16 +1005,16 @@
       <c r="L6" s="1">
         <v>66.741</v>
       </c>
-      <c r="M6" s="18">
+      <c r="M6" s="17">
         <v>4</v>
       </c>
-      <c r="N6" s="11">
+      <c r="N6" s="10">
         <v>1.7090000000000001</v>
       </c>
-      <c r="O6" s="19">
+      <c r="O6" s="18">
         <v>28.664999999999999</v>
       </c>
-      <c r="P6" s="11">
+      <c r="P6" s="10">
         <f t="shared" si="0"/>
         <v>49.851530000000004</v>
       </c>
@@ -1023,9 +1030,9 @@
         <v>18</v>
       </c>
       <c r="D7" s="13">
-        <v>2375.08</v>
-      </c>
-      <c r="E7" s="14">
+        <v>2558.9969999999998</v>
+      </c>
+      <c r="E7" s="13">
         <v>2558.9969999999998</v>
       </c>
       <c r="F7" s="5">
@@ -1043,20 +1050,20 @@
       <c r="K7" s="1">
         <v>21.2</v>
       </c>
-      <c r="L7" s="10">
+      <c r="L7" s="9">
         <f t="shared" ref="L7:L14" si="1">J7*29.17</f>
         <v>67.411870000000008</v>
       </c>
-      <c r="M7" s="18">
+      <c r="M7" s="17">
         <v>29</v>
       </c>
-      <c r="N7" s="11">
+      <c r="N7" s="10">
         <v>1.5980000000000001</v>
       </c>
-      <c r="O7" s="19">
+      <c r="O7" s="18">
         <v>30.655000000000001</v>
       </c>
-      <c r="P7" s="11">
+      <c r="P7" s="10">
         <f t="shared" si="0"/>
         <v>46.613660000000003</v>
       </c>
@@ -1071,9 +1078,11 @@
       <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="10"/>
+      <c r="D8" s="13">
+        <v>1902.38</v>
+      </c>
       <c r="E8" s="13">
-        <v>1902.347</v>
+        <v>1902.38</v>
       </c>
       <c r="F8" s="5">
         <v>1902.38</v>
@@ -1090,20 +1099,20 @@
       <c r="K8" s="1">
         <v>22.59</v>
       </c>
-      <c r="L8" s="10">
+      <c r="L8" s="9">
         <f t="shared" si="1"/>
         <v>63.269730000000003</v>
       </c>
-      <c r="M8" s="18">
+      <c r="M8" s="17">
         <v>26</v>
       </c>
-      <c r="N8" s="11">
+      <c r="N8" s="10">
         <v>1.6240000000000001</v>
       </c>
-      <c r="O8" s="19">
+      <c r="O8" s="18">
         <v>30.164999999999999</v>
       </c>
-      <c r="P8" s="11">
+      <c r="P8" s="10">
         <f t="shared" si="0"/>
         <v>47.372080000000004</v>
       </c>
@@ -1118,18 +1127,20 @@
       <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="13">
         <v>2764.7620000000002</v>
       </c>
-      <c r="E9" s="10"/>
+      <c r="E9" s="13">
+        <v>2764.7620000000002</v>
+      </c>
       <c r="F9" s="5">
         <v>2764.7620000000002</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I9" s="9">
-        <v>43313</v>
+      <c r="I9" s="22">
+        <v>1</v>
       </c>
       <c r="J9" s="1">
         <v>2.2360000000000002</v>
@@ -1137,20 +1148,20 @@
       <c r="K9" s="1">
         <v>21.914999999999999</v>
       </c>
-      <c r="L9" s="10">
+      <c r="L9" s="9">
         <f t="shared" si="1"/>
         <v>65.224120000000013</v>
       </c>
-      <c r="M9" s="18">
+      <c r="M9" s="17">
         <v>31</v>
       </c>
-      <c r="N9" s="11">
+      <c r="N9" s="10">
         <v>1.5920000000000001</v>
       </c>
-      <c r="O9" s="19">
+      <c r="O9" s="18">
         <v>30.785</v>
       </c>
-      <c r="P9" s="11">
+      <c r="P9" s="10">
         <f t="shared" si="0"/>
         <v>46.438640000000007</v>
       </c>
@@ -1165,8 +1176,10 @@
       <c r="C10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="14">
+      <c r="D10" s="13">
+        <v>2473.3829999999998</v>
+      </c>
+      <c r="E10" s="13">
         <v>2473.3829999999998</v>
       </c>
       <c r="F10" s="5">
@@ -1184,20 +1197,20 @@
       <c r="K10" s="1">
         <v>22.18</v>
       </c>
-      <c r="L10" s="10">
+      <c r="L10" s="9">
         <f t="shared" si="1"/>
         <v>64.436530000000005</v>
       </c>
-      <c r="M10" s="18">
+      <c r="M10" s="17">
         <v>28</v>
       </c>
-      <c r="N10" s="11">
+      <c r="N10" s="10">
         <v>1.6419999999999999</v>
       </c>
-      <c r="O10" s="19">
+      <c r="O10" s="18">
         <v>29.85</v>
       </c>
-      <c r="P10" s="11">
+      <c r="P10" s="10">
         <f t="shared" si="0"/>
         <v>47.89714</v>
       </c>
@@ -1212,8 +1225,12 @@
       <c r="C11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
+      <c r="D11" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="13">
+        <v>1697.8689999999999</v>
+      </c>
       <c r="F11" s="5">
         <v>1697.8689999999999</v>
       </c>
@@ -1229,20 +1246,20 @@
       <c r="K11" s="1">
         <v>21.88</v>
       </c>
-      <c r="L11" s="10">
+      <c r="L11" s="9">
         <f t="shared" si="1"/>
         <v>65.311629999999994</v>
       </c>
-      <c r="M11" s="18">
+      <c r="M11" s="17">
         <v>25</v>
       </c>
-      <c r="N11" s="11">
+      <c r="N11" s="10">
         <v>1.6990000000000001</v>
       </c>
-      <c r="O11" s="19">
+      <c r="O11" s="18">
         <v>28.84</v>
       </c>
-      <c r="P11" s="11">
+      <c r="P11" s="10">
         <f t="shared" si="0"/>
         <v>49.559830000000005</v>
       </c>
@@ -1257,8 +1274,10 @@
       <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="14">
+      <c r="D12" s="13">
+        <v>1420.316</v>
+      </c>
+      <c r="E12" s="13">
         <v>1420.316</v>
       </c>
       <c r="F12" s="5">
@@ -1276,20 +1295,20 @@
       <c r="K12" s="1">
         <v>22.15</v>
       </c>
-      <c r="L12" s="10">
+      <c r="L12" s="9">
         <f t="shared" si="1"/>
         <v>64.524040000000014</v>
       </c>
-      <c r="M12" s="18">
+      <c r="M12" s="17">
         <v>30</v>
       </c>
-      <c r="N12" s="11">
+      <c r="N12" s="10">
         <v>1.42</v>
       </c>
-      <c r="O12" s="19">
+      <c r="O12" s="18">
         <v>34.5</v>
       </c>
-      <c r="P12" s="11">
+      <c r="P12" s="10">
         <f t="shared" si="0"/>
         <v>41.421399999999998</v>
       </c>
@@ -1304,8 +1323,12 @@
       <c r="C13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
+      <c r="D13" s="12">
+        <v>1060.83</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>44</v>
+      </c>
       <c r="F13" s="5">
         <v>1060.825</v>
       </c>
@@ -1321,20 +1344,20 @@
       <c r="K13" s="1">
         <v>23.225000000000001</v>
       </c>
-      <c r="L13" s="10">
+      <c r="L13" s="9">
         <f t="shared" si="1"/>
         <v>61.548699999999997</v>
       </c>
-      <c r="M13" s="18">
+      <c r="M13" s="17">
         <v>27</v>
       </c>
-      <c r="N13" s="11">
+      <c r="N13" s="10">
         <v>1.48</v>
       </c>
-      <c r="O13" s="19">
+      <c r="O13" s="18">
         <v>33.115000000000002</v>
       </c>
-      <c r="P13" s="11">
+      <c r="P13" s="10">
         <f t="shared" si="0"/>
         <v>43.171600000000005</v>
       </c>
@@ -1349,8 +1372,12 @@
       <c r="C14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
+      <c r="D14" s="12">
+        <v>810.16800000000001</v>
+      </c>
+      <c r="E14" s="12">
+        <v>812.09</v>
+      </c>
       <c r="F14" s="5">
         <v>812.09299999999996</v>
       </c>
@@ -1366,20 +1393,20 @@
       <c r="K14" s="1">
         <v>23.82</v>
       </c>
-      <c r="L14" s="10">
+      <c r="L14" s="9">
         <f t="shared" si="1"/>
         <v>60.002690000000001</v>
       </c>
-      <c r="M14" s="18">
+      <c r="M14" s="17">
         <v>4</v>
       </c>
-      <c r="N14" s="11">
+      <c r="N14" s="10">
         <v>1.5620000000000001</v>
       </c>
-      <c r="O14" s="19">
+      <c r="O14" s="18">
         <v>31.364999999999998</v>
       </c>
-      <c r="P14" s="11">
+      <c r="P14" s="10">
         <f t="shared" si="0"/>
         <v>45.563540000000003</v>
       </c>
@@ -1394,10 +1421,12 @@
       <c r="C15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="13">
         <v>775.89331000000016</v>
       </c>
-      <c r="E15" s="10"/>
+      <c r="E15" s="13">
+        <v>775.89300000000003</v>
+      </c>
       <c r="F15" s="5">
         <v>775.89300000000003</v>
       </c>
@@ -1405,22 +1434,22 @@
         <v>20</v>
       </c>
       <c r="I15" s="1"/>
-      <c r="J15" s="10">
+      <c r="J15" s="9">
         <f>SUM(J3:J14)</f>
         <v>26.599</v>
       </c>
       <c r="K15" s="1"/>
-      <c r="L15" s="14">
+      <c r="L15" s="13">
         <f>SUM(L3:L14)</f>
         <v>775.89331000000016</v>
       </c>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11">
+      <c r="M15" s="10"/>
+      <c r="N15" s="10">
         <f>SUM(N3:N14)</f>
         <v>19.591000000000001</v>
       </c>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11">
+      <c r="O15" s="10"/>
+      <c r="P15" s="23">
         <f>SUM(P3:P14)</f>
         <v>571.46947</v>
       </c>
@@ -1435,10 +1464,10 @@
       <c r="C16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D16" s="13">
         <v>571.46900000000005</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="13">
         <v>571.46900000000005</v>
       </c>
       <c r="F16" s="5">
@@ -1455,8 +1484,12 @@
       <c r="C17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
+      <c r="D17" s="13">
+        <v>561.37699999999995</v>
+      </c>
+      <c r="E17" s="13">
+        <v>561.37699999999995</v>
+      </c>
       <c r="F17" s="5">
         <v>561.37699999999995</v>
       </c>
@@ -1471,10 +1504,10 @@
       <c r="C18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="13">
-        <v>489.09331041653002</v>
-      </c>
-      <c r="E18" s="14">
+      <c r="D18" s="12">
+        <v>486.20600000000002</v>
+      </c>
+      <c r="E18" s="13">
         <v>485.59300000000002</v>
       </c>
       <c r="F18" s="5">
@@ -1487,15 +1520,15 @@
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
-      <c r="D19" s="15">
+      <c r="D19" s="14">
         <f>SUM(D2:D18)</f>
-        <v>26477.32035459701</v>
-      </c>
-      <c r="E19" s="15">
+        <v>34886.829310000001</v>
+      </c>
+      <c r="E19" s="14">
         <f>SUM(E2:E18)</f>
-        <v>28901.333923935814</v>
-      </c>
-      <c r="F19" s="20">
+        <v>35513.393999999986</v>
+      </c>
+      <c r="F19" s="19">
         <v>36585.567999999999</v>
       </c>
     </row>
@@ -1512,7 +1545,7 @@
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="15" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1520,29 +1553,29 @@
       <c r="A23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="21" t="s">
-        <v>41</v>
+      <c r="D23" s="20" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D24" s="22" t="s">
-        <v>42</v>
+      <c r="D24" s="21" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="16" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1550,7 +1583,7 @@
       <c r="A26" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="15" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1558,19 +1591,23 @@
       <c r="A27" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="17"/>
+      <c r="B27" s="15" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="17"/>
+      <c r="B28" s="15" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="15" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1578,31 +1615,39 @@
       <c r="A30" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="17"/>
+      <c r="B30" s="15" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="17"/>
+      <c r="B31" s="16" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="17"/>
+      <c r="B32" s="16" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B33" s="17"/>
+      <c r="B33" s="16" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="15" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correción de Pol. Closed #70, closed #72. Añadidos finalmente los resultados de Josep. TOTAL CORRECTO = 36585.568
</commit_message>
<xml_diff>
--- a/Zara.Reto0/ZaraCalculos.xlsx
+++ b/Zara.Reto0/ZaraCalculos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="46">
   <si>
     <t>Nombre</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Resultado de mi código</t>
   </si>
 </sst>
 </file>
@@ -259,7 +262,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -305,6 +308,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -408,7 +423,7 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2"/>
@@ -428,11 +443,13 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="7" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="8"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="4" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="6" xfId="8" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="6" xfId="8" applyFill="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Bad" xfId="4" builtinId="27"/>
@@ -724,7 +741,7 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -734,7 +751,7 @@
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="20.44140625" customWidth="1"/>
-    <col min="6" max="6" width="15.21875" customWidth="1"/>
+    <col min="6" max="6" width="22.109375" customWidth="1"/>
     <col min="8" max="10" width="13.21875" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
     <col min="12" max="12" width="11.109375" customWidth="1"/>
@@ -1139,7 +1156,7 @@
       <c r="H9" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I9" s="22">
+      <c r="I9" s="21">
         <v>1</v>
       </c>
       <c r="J9" s="1">
@@ -1323,8 +1340,8 @@
       <c r="C13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="12">
-        <v>1060.83</v>
+      <c r="D13" s="13">
+        <v>1060.825</v>
       </c>
       <c r="E13" s="12" t="s">
         <v>44</v>
@@ -1375,8 +1392,8 @@
       <c r="D14" s="12">
         <v>810.16800000000001</v>
       </c>
-      <c r="E14" s="12">
-        <v>812.09</v>
+      <c r="E14" s="13">
+        <v>812.09299999999996</v>
       </c>
       <c r="F14" s="5">
         <v>812.09299999999996</v>
@@ -1449,7 +1466,7 @@
         <v>19.591000000000001</v>
       </c>
       <c r="O15" s="10"/>
-      <c r="P15" s="23">
+      <c r="P15" s="22">
         <f>SUM(P3:P14)</f>
         <v>571.46947</v>
       </c>
@@ -1521,15 +1538,16 @@
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="14">
-        <f>SUM(D2:D18)</f>
-        <v>34886.829310000001</v>
+        <f>SUM(D2,F3,D4:D10,F11,D12:D13,F14,D15:D17,F18)</f>
+        <v>36585.569309999992</v>
       </c>
       <c r="E19" s="14">
-        <f>SUM(E2:E18)</f>
-        <v>35513.393999999986</v>
-      </c>
-      <c r="F19" s="19">
-        <v>36585.567999999999</v>
+        <f>SUM(E2,E3,F4,E5:E12,F13,E14:E18)</f>
+        <v>36585.568999999989</v>
+      </c>
+      <c r="F19" s="23">
+        <f>SUM(F2:F18)</f>
+        <v>36585.568999999989</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
@@ -1556,22 +1574,28 @@
       <c r="B23" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="D23" s="19" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F23" s="24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B24" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D24" s="21" t="s">
+      <c r="D24" s="20" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F24" s="25">
+        <v>36585.567999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>10</v>
       </c>
@@ -1631,7 +1655,7 @@
       <c r="A32" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="15" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ISSUE #81 a mitad. No he encontrado solución aún al problema de FLYWAY DB
</commit_message>
<xml_diff>
--- a/Zara.Reto0/ZaraCalculos.xlsx
+++ b/Zara.Reto0/ZaraCalculos.xlsx
@@ -735,7 +735,7 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1540,8 +1540,7 @@
         <v>36563.516999999993</v>
       </c>
       <c r="F19" s="23">
-        <f>SUM(F2:F18)</f>
-        <v>36585.568999999989</v>
+        <v>36585.567999999999</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>

</xml_diff>